<commit_message>
catch-all route correctly arranged
</commit_message>
<xml_diff>
--- a/UserAttendance.xlsx
+++ b/UserAttendance.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>fullname</t>
   </si>
@@ -41,6 +41,15 @@
   </si>
   <si>
     <t>NPC Headquaters</t>
+  </si>
+  <si>
+    <t>19:26:53 GMT+0100 (West Africa Standard Time)</t>
+  </si>
+  <si>
+    <t>Fri Jun 07 2024</t>
+  </si>
+  <si>
+    <t>19:26:54 GMT+0100 (West Africa Standard Time)</t>
   </si>
 </sst>
 </file>
@@ -417,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -451,6 +460,34 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>